<commit_message>
updated lab5 3-rd task
</commit_message>
<xml_diff>
--- a/lab5/task3/solutions_table_2.xlsx
+++ b/lab5/task3/solutions_table_2.xlsx
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,8 @@
     <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="9" width="4.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" customWidth="1"/>
     <col min="10" max="10" width="4.28515625" customWidth="1"/>
     <col min="11" max="11" width="5" customWidth="1"/>
     <col min="12" max="12" width="4.42578125" customWidth="1"/>
@@ -2480,31 +2481,31 @@
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K30" s="13" t="s">
+      <c r="C30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="18" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>